<commit_message>
updated the 2N3904 npn transistor footprint
</commit_message>
<xml_diff>
--- a/v1.0/WiTooth_v1P0.xlsx
+++ b/v1.0/WiTooth_v1P0.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\PCB Design\WiTooth\v1.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="WiTooth_v1P0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -991,6 +996,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1038,7 +1046,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1073,7 +1081,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1282,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,28 +2556,28 @@
         <v>108</v>
       </c>
       <c r="I26" s="8">
-        <v>192.5</v>
+        <v>90</v>
       </c>
       <c r="J26" s="8">
-        <v>178.5</v>
+        <v>85</v>
       </c>
       <c r="K26" s="8">
-        <v>168.7</v>
+        <v>80</v>
       </c>
       <c r="L26" s="8">
-        <v>162.4</v>
+        <v>70</v>
       </c>
       <c r="N26">
         <f t="shared" si="0"/>
-        <v>192.5</v>
+        <v>90</v>
       </c>
       <c r="O26">
         <f t="shared" si="1"/>
-        <v>178.5</v>
+        <v>85</v>
       </c>
       <c r="P26">
         <f t="shared" si="2"/>
-        <v>162.4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2673,15 +2681,26 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15">
         <f xml:space="preserve"> SUM(N2:N28)</f>
-        <v>1113.1399999999999</v>
+        <v>1010.64</v>
       </c>
       <c r="O31" s="15">
         <f>SUM(O2:O28)</f>
-        <v>969.4</v>
+        <v>875.9</v>
       </c>
       <c r="P31" s="15">
         <f>SUM(P2:P28)</f>
-        <v>895.75</v>
+        <v>803.35</v>
+      </c>
+    </row>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <f>N31+N33+150</f>
+        <v>1510.6399999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>